<commit_message>
changed date format of demo data to match instructions format
</commit_message>
<xml_diff>
--- a/demo_data/timeoftips.xlsx
+++ b/demo_data/timeoftips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/rainfall_flow_calculator_shiny/demo_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/PartTimers/Nick Lombardo/Bioretention/rainfall_flow_analysis/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{7E0DBA5F-C6BC-4A22-A987-792D5A2998D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F4B2605-A818-4D7B-BF06-1BC9B8111C33}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{7E0DBA5F-C6BC-4A22-A987-792D5A2998D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E002CDF-B621-426E-A24D-310D3F2DD6A9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -80,13 +80,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,6 +640,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -934,103 +941,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
+      <c r="A1" s="2"/>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1043,18 +1050,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B346"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1062,7 +1067,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>18308.707638888889</v>
       </c>
       <c r="B2">
@@ -1070,7 +1075,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>18308.708449074071</v>
       </c>
       <c r="B3">
@@ -1078,7 +1083,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>18308.709143518521</v>
       </c>
       <c r="B4">
@@ -1086,7 +1091,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>18308.709953703699</v>
       </c>
       <c r="B5">
@@ -1094,7 +1099,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>18308.71157407407</v>
       </c>
       <c r="B6">
@@ -1102,7 +1107,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>18308.71261574074</v>
       </c>
       <c r="B7">
@@ -1110,7 +1115,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>18308.713773148149</v>
       </c>
       <c r="B8">
@@ -1118,7 +1123,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
         <v>18308.714930555561</v>
       </c>
       <c r="B9">
@@ -1126,7 +1131,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="4">
         <v>18308.71631944444</v>
       </c>
       <c r="B10">
@@ -1134,7 +1139,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="4">
         <v>18308.717245370372</v>
       </c>
       <c r="B11">
@@ -1142,7 +1147,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="4">
         <v>18308.720717592591</v>
       </c>
       <c r="B12">
@@ -1150,7 +1155,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="4">
         <v>18308.721412037041</v>
       </c>
       <c r="B13">
@@ -1158,7 +1163,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="4">
         <v>18308.721874999999</v>
       </c>
       <c r="B14">
@@ -1166,7 +1171,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="4">
         <v>18308.726041666669</v>
       </c>
       <c r="B15">
@@ -1174,7 +1179,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="4">
         <v>18315.895949074071</v>
       </c>
       <c r="B16">
@@ -1182,7 +1187,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="4">
         <v>18317.18136574074</v>
       </c>
       <c r="B17">
@@ -1190,7 +1195,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="4">
         <v>18317.183449074069</v>
       </c>
       <c r="B18">
@@ -1198,7 +1203,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="4">
         <v>18317.186921296299</v>
       </c>
       <c r="B19">
@@ -1206,7 +1211,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="4">
         <v>18317.192824074071</v>
       </c>
       <c r="B20">
@@ -1214,7 +1219,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="4">
         <v>18317.248842592591</v>
       </c>
       <c r="B21">
@@ -1222,7 +1227,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="4">
         <v>18317.251504629628</v>
       </c>
       <c r="B22">
@@ -1230,7 +1235,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="4">
         <v>18317.255208333328</v>
       </c>
       <c r="B23">
@@ -1238,7 +1243,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="4">
         <v>18317.25949074074</v>
       </c>
       <c r="B24">
@@ -1246,7 +1251,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="4">
         <v>18317.26701388889</v>
       </c>
       <c r="B25">
@@ -1254,7 +1259,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="4">
         <v>18317.281018518519</v>
       </c>
       <c r="B26">
@@ -1262,7 +1267,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="4">
         <v>18317.308449074069</v>
       </c>
       <c r="B27">
@@ -1270,7 +1275,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="4">
         <v>18317.323958333331</v>
       </c>
       <c r="B28">
@@ -1278,7 +1283,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="4">
         <v>18317.417824074069</v>
       </c>
       <c r="B29">
@@ -1286,7 +1291,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="4">
         <v>18317.42662037037</v>
       </c>
       <c r="B30">
@@ -1294,7 +1299,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="4">
         <v>18317.432986111111</v>
       </c>
       <c r="B31">
@@ -1302,7 +1307,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="4">
         <v>18317.4412037037</v>
       </c>
       <c r="B32">
@@ -1310,7 +1315,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="4">
         <v>18317.453703703701</v>
       </c>
       <c r="B33">
@@ -1318,7 +1323,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="4">
         <v>18317.539236111112</v>
       </c>
       <c r="B34">
@@ -1326,7 +1331,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="4">
         <v>18317.53981481482</v>
       </c>
       <c r="B35">
@@ -1334,7 +1339,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="4">
         <v>18317.540277777782</v>
       </c>
       <c r="B36">
@@ -1342,7 +1347,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="4">
         <v>18317.541203703699</v>
       </c>
       <c r="B37">
@@ -1350,7 +1355,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="4">
         <v>18317.542592592588</v>
       </c>
       <c r="B38">
@@ -1358,7 +1363,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="4">
         <v>18317.54444444444</v>
       </c>
       <c r="B39">
@@ -1366,7 +1371,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="A40" s="4">
         <v>18317.862847222219</v>
       </c>
       <c r="B40">
@@ -1374,7 +1379,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="4">
         <v>18317.86689814815</v>
       </c>
       <c r="B41">
@@ -1382,7 +1387,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="4">
         <v>18317.876273148151</v>
       </c>
       <c r="B42">
@@ -1390,7 +1395,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="4">
         <v>18317.89675925926</v>
       </c>
       <c r="B43">
@@ -1398,7 +1403,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="4">
         <v>18317.915509259259</v>
       </c>
       <c r="B44">
@@ -1406,7 +1411,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="4">
         <v>18317.925694444439</v>
       </c>
       <c r="B45">
@@ -1414,7 +1419,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="4">
         <v>18317.93171296296</v>
       </c>
       <c r="B46">
@@ -1422,7 +1427,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="4">
         <v>18317.935763888891</v>
       </c>
       <c r="B47">
@@ -1430,7 +1435,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="4">
         <v>18318.290972222221</v>
       </c>
       <c r="B48">
@@ -1438,7 +1443,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="A49" s="4">
         <v>18318.609143518519</v>
       </c>
       <c r="B49">
@@ -1446,7 +1451,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="A50" s="4">
         <v>18318.663888888888</v>
       </c>
       <c r="B50">
@@ -1454,7 +1459,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="A51" s="4">
         <v>18318.673958333329</v>
       </c>
       <c r="B51">
@@ -1462,7 +1467,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="A52" s="4">
         <v>18318.68240740741</v>
       </c>
       <c r="B52">
@@ -1470,7 +1475,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="4">
         <v>18318.692824074071</v>
       </c>
       <c r="B53">
@@ -1478,7 +1483,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="A54" s="4">
         <v>18318.708101851851</v>
       </c>
       <c r="B54">
@@ -1486,7 +1491,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="4">
         <v>18318.725115740741</v>
       </c>
       <c r="B55">
@@ -1494,7 +1499,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="A56" s="4">
         <v>18318.735532407409</v>
       </c>
       <c r="B56">
@@ -1502,7 +1507,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="4">
         <v>18318.745833333331</v>
       </c>
       <c r="B57">
@@ -1510,7 +1515,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="A58" s="4">
         <v>18318.753819444439</v>
       </c>
       <c r="B58">
@@ -1518,7 +1523,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="A59" s="4">
         <v>18318.792939814819</v>
       </c>
       <c r="B59">
@@ -1526,7 +1531,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="A60" s="4">
         <v>18319.127083333329</v>
       </c>
       <c r="B60">
@@ -1534,7 +1539,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="4">
         <v>18319.131944444449</v>
       </c>
       <c r="B61">
@@ -1542,7 +1547,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="A62" s="4">
         <v>18319.133217592589</v>
       </c>
       <c r="B62">
@@ -1550,7 +1555,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="A63" s="4">
         <v>18319.134259259259</v>
       </c>
       <c r="B63">
@@ -1558,7 +1563,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="4">
         <v>18319.136342592588</v>
       </c>
       <c r="B64">
@@ -1566,7 +1571,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="A65" s="4">
         <v>18319.137500000001</v>
       </c>
       <c r="B65">
@@ -1574,7 +1579,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="A66" s="4">
         <v>18319.138541666671</v>
       </c>
       <c r="B66">
@@ -1582,7 +1587,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="4">
         <v>18319.139467592591</v>
       </c>
       <c r="B67">
@@ -1590,7 +1595,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="A68" s="4">
         <v>18319.140393518519</v>
       </c>
       <c r="B68">
@@ -1598,7 +1603,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="A69" s="4">
         <v>18319.14131944445</v>
       </c>
       <c r="B69">
@@ -1606,7 +1611,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="A70" s="4">
         <v>18319.14201388889</v>
       </c>
       <c r="B70">
@@ -1614,7 +1619,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="A71" s="4">
         <v>18319.142824074079</v>
       </c>
       <c r="B71">
@@ -1622,7 +1627,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="4">
         <v>18319.14340277778</v>
       </c>
       <c r="B72">
@@ -1630,7 +1635,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="A73" s="4">
         <v>18319.144212962961</v>
       </c>
       <c r="B73">
@@ -1638,7 +1643,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="A74" s="4">
         <v>18319.145254629631</v>
       </c>
       <c r="B74">
@@ -1646,7 +1651,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="A75" s="4">
         <v>18319.14606481481</v>
       </c>
       <c r="B75">
@@ -1654,7 +1659,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="A76" s="4">
         <v>18319.148611111112</v>
       </c>
       <c r="B76">
@@ -1662,7 +1667,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="A77" s="4">
         <v>18319.151273148149</v>
       </c>
       <c r="B77">
@@ -1670,7 +1675,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="A78" s="4">
         <v>18319.15393518519</v>
       </c>
       <c r="B78">
@@ -1678,7 +1683,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="A79" s="4">
         <v>18319.155787037042</v>
       </c>
       <c r="B79">
@@ -1686,7 +1691,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="4">
         <v>18319.15763888889</v>
       </c>
       <c r="B80">
@@ -1694,7 +1699,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="A81" s="4">
         <v>18319.159143518518</v>
       </c>
       <c r="B81">
@@ -1702,7 +1707,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="4">
         <v>18319.161574074071</v>
       </c>
       <c r="B82">
@@ -1710,7 +1715,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="A83" s="4">
         <v>18319.163888888888</v>
       </c>
       <c r="B83">
@@ -1718,7 +1723,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="A84" s="4">
         <v>18319.165972222221</v>
       </c>
       <c r="B84">
@@ -1726,7 +1731,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="A85" s="4">
         <v>18319.1681712963</v>
       </c>
       <c r="B85">
@@ -1734,7 +1739,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+      <c r="A86" s="4">
         <v>18319.171296296299</v>
       </c>
       <c r="B86">
@@ -1742,7 +1747,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="A87" s="4">
         <v>18319.177430555559</v>
       </c>
       <c r="B87">
@@ -1750,7 +1755,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="A88" s="4">
         <v>18319.181597222221</v>
       </c>
       <c r="B88">
@@ -1758,7 +1763,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="A89" s="4">
         <v>18319.185879629629</v>
       </c>
       <c r="B89">
@@ -1766,7 +1771,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="A90" s="4">
         <v>18319.189467592591</v>
       </c>
       <c r="B90">
@@ -1774,7 +1779,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="A91" s="4">
         <v>18319.19259259259</v>
       </c>
       <c r="B91">
@@ -1782,7 +1787,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="A92" s="4">
         <v>18319.19467592593</v>
       </c>
       <c r="B92">
@@ -1790,7 +1795,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+      <c r="A93" s="4">
         <v>18319.19699074074</v>
       </c>
       <c r="B93">
@@ -1798,7 +1803,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+      <c r="A94" s="4">
         <v>18319.199884259258</v>
       </c>
       <c r="B94">
@@ -1806,7 +1811,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="A95" s="4">
         <v>18319.203125</v>
       </c>
       <c r="B95">
@@ -1814,7 +1819,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="A96" s="4">
         <v>18319.209837962961</v>
       </c>
       <c r="B96">
@@ -1822,7 +1827,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="A97" s="4">
         <v>18319.21770833333</v>
       </c>
       <c r="B97">
@@ -1830,7 +1835,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="A98" s="4">
         <v>18319.220833333329</v>
       </c>
       <c r="B98">
@@ -1838,7 +1843,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="A99" s="4">
         <v>18319.223611111109</v>
       </c>
       <c r="B99">
@@ -1846,7 +1851,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="A100" s="4">
         <v>18319.227083333331</v>
       </c>
       <c r="B100">
@@ -1854,7 +1859,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+      <c r="A101" s="4">
         <v>18319.231712962959</v>
       </c>
       <c r="B101">
@@ -1862,7 +1867,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+      <c r="A102" s="4">
         <v>18319.234259259261</v>
       </c>
       <c r="B102">
@@ -1870,7 +1875,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+      <c r="A103" s="4">
         <v>18319.237268518518</v>
       </c>
       <c r="B103">
@@ -1878,7 +1883,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+      <c r="A104" s="4">
         <v>18319.240624999999</v>
       </c>
       <c r="B104">
@@ -1886,7 +1891,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
+      <c r="A105" s="4">
         <v>18319.245486111111</v>
       </c>
       <c r="B105">
@@ -1894,7 +1899,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
+      <c r="A106" s="4">
         <v>18319.24895833333</v>
       </c>
       <c r="B106">
@@ -1902,7 +1907,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
+      <c r="A107" s="4">
         <v>18319.252893518518</v>
       </c>
       <c r="B107">
@@ -1910,7 +1915,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+      <c r="A108" s="4">
         <v>18319.256828703699</v>
       </c>
       <c r="B108">
@@ -1918,7 +1923,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+      <c r="A109" s="4">
         <v>18319.260069444441</v>
       </c>
       <c r="B109">
@@ -1926,7 +1931,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+      <c r="A110" s="4">
         <v>18319.26319444444</v>
       </c>
       <c r="B110">
@@ -1934,7 +1939,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+      <c r="A111" s="4">
         <v>18319.26666666667</v>
       </c>
       <c r="B111">
@@ -1942,7 +1947,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+      <c r="A112" s="4">
         <v>18319.272222222218</v>
       </c>
       <c r="B112">
@@ -1950,7 +1955,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+      <c r="A113" s="4">
         <v>18319.27476851852</v>
       </c>
       <c r="B113">
@@ -1958,7 +1963,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+      <c r="A114" s="4">
         <v>18319.278009259258</v>
       </c>
       <c r="B114">
@@ -1966,7 +1971,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+      <c r="A115" s="4">
         <v>18319.28194444445</v>
       </c>
       <c r="B115">
@@ -1974,7 +1979,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+      <c r="A116" s="4">
         <v>18319.2849537037</v>
       </c>
       <c r="B116">
@@ -1982,7 +1987,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+      <c r="A117" s="4">
         <v>18319.289004629631</v>
       </c>
       <c r="B117">
@@ -1990,7 +1995,7 @@
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+      <c r="A118" s="4">
         <v>18319.292245370369</v>
       </c>
       <c r="B118">
@@ -1998,7 +2003,7 @@
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+      <c r="A119" s="4">
         <v>18319.295023148152</v>
       </c>
       <c r="B119">
@@ -2006,7 +2011,7 @@
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+      <c r="A120" s="4">
         <v>18319.298379629628</v>
       </c>
       <c r="B120">
@@ -2014,7 +2019,7 @@
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+      <c r="A121" s="4">
         <v>18319.302083333328</v>
       </c>
       <c r="B121">
@@ -2022,7 +2027,7 @@
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+      <c r="A122" s="4">
         <v>18319.30497685185</v>
       </c>
       <c r="B122">
@@ -2030,7 +2035,7 @@
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+      <c r="A123" s="4">
         <v>18319.306828703699</v>
       </c>
       <c r="B123">
@@ -2038,7 +2043,7 @@
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+      <c r="A124" s="4">
         <v>18319.309259259258</v>
       </c>
       <c r="B124">
@@ -2046,7 +2051,7 @@
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+      <c r="A125" s="4">
         <v>18319.31157407408</v>
       </c>
       <c r="B125">
@@ -2054,7 +2059,7 @@
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+      <c r="A126" s="4">
         <v>18319.31342592592</v>
       </c>
       <c r="B126">
@@ -2062,7 +2067,7 @@
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+      <c r="A127" s="4">
         <v>18319.315624999999</v>
       </c>
       <c r="B127">
@@ -2070,7 +2075,7 @@
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+      <c r="A128" s="4">
         <v>18319.317476851851</v>
       </c>
       <c r="B128">
@@ -2078,7 +2083,7 @@
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="2">
+      <c r="A129" s="4">
         <v>18319.319097222218</v>
       </c>
       <c r="B129">
@@ -2086,7 +2091,7 @@
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2">
+      <c r="A130" s="4">
         <v>18319.321296296301</v>
       </c>
       <c r="B130">
@@ -2094,7 +2099,7 @@
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="2">
+      <c r="A131" s="4">
         <v>18319.323611111111</v>
       </c>
       <c r="B131">
@@ -2102,7 +2107,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="2">
+      <c r="A132" s="4">
         <v>18319.326157407409</v>
       </c>
       <c r="B132">
@@ -2110,7 +2115,7 @@
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2">
+      <c r="A133" s="4">
         <v>18319.32777777778</v>
       </c>
       <c r="B133">
@@ -2118,7 +2123,7 @@
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="2">
+      <c r="A134" s="4">
         <v>18319.328935185189</v>
       </c>
       <c r="B134">
@@ -2126,7 +2131,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2">
+      <c r="A135" s="4">
         <v>18319.330208333329</v>
       </c>
       <c r="B135">
@@ -2134,7 +2139,7 @@
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="2">
+      <c r="A136" s="4">
         <v>18319.331597222219</v>
       </c>
       <c r="B136">
@@ -2142,7 +2147,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="2">
+      <c r="A137" s="4">
         <v>18319.333333333328</v>
       </c>
       <c r="B137">
@@ -2150,7 +2155,7 @@
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="2">
+      <c r="A138" s="4">
         <v>18319.335069444449</v>
       </c>
       <c r="B138">
@@ -2158,7 +2163,7 @@
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="2">
+      <c r="A139" s="4">
         <v>18319.336805555551</v>
       </c>
       <c r="B139">
@@ -2166,7 +2171,7 @@
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="2">
+      <c r="A140" s="4">
         <v>18319.338773148149</v>
       </c>
       <c r="B140">
@@ -2174,7 +2179,7 @@
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2">
+      <c r="A141" s="4">
         <v>18319.341087962959</v>
       </c>
       <c r="B141">
@@ -2182,7 +2187,7 @@
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2">
+      <c r="A142" s="4">
         <v>18319.342939814811</v>
       </c>
       <c r="B142">
@@ -2190,7 +2195,7 @@
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="2">
+      <c r="A143" s="4">
         <v>18319.344907407409</v>
       </c>
       <c r="B143">
@@ -2198,7 +2203,7 @@
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="2">
+      <c r="A144" s="4">
         <v>18319.346643518518</v>
       </c>
       <c r="B144">
@@ -2206,7 +2211,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="2">
+      <c r="A145" s="4">
         <v>18319.348958333328</v>
       </c>
       <c r="B145">
@@ -2214,7 +2219,7 @@
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
+      <c r="A146" s="4">
         <v>18319.353125000001</v>
       </c>
       <c r="B146">
@@ -2222,7 +2227,7 @@
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="2">
+      <c r="A147" s="4">
         <v>18319.357407407409</v>
       </c>
       <c r="B147">
@@ -2230,7 +2235,7 @@
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="2">
+      <c r="A148" s="4">
         <v>18319.361111111109</v>
       </c>
       <c r="B148">
@@ -2238,7 +2243,7 @@
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="2">
+      <c r="A149" s="4">
         <v>18319.364236111109</v>
       </c>
       <c r="B149">
@@ -2246,7 +2251,7 @@
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="2">
+      <c r="A150" s="4">
         <v>18319.367245370369</v>
       </c>
       <c r="B150">
@@ -2254,7 +2259,7 @@
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="2">
+      <c r="A151" s="4">
         <v>18319.370486111111</v>
       </c>
       <c r="B151">
@@ -2262,7 +2267,7 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="2">
+      <c r="A152" s="4">
         <v>18319.373495370372</v>
       </c>
       <c r="B152">
@@ -2270,7 +2275,7 @@
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="2">
+      <c r="A153" s="4">
         <v>18319.376851851848</v>
       </c>
       <c r="B153">
@@ -2278,7 +2283,7 @@
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="2">
+      <c r="A154" s="4">
         <v>18319.38009259259</v>
       </c>
       <c r="B154">
@@ -2286,7 +2291,7 @@
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="2">
+      <c r="A155" s="4">
         <v>18319.383912037039</v>
       </c>
       <c r="B155">
@@ -2294,7 +2299,7 @@
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="2">
+      <c r="A156" s="4">
         <v>18319.38831018519</v>
       </c>
       <c r="B156">
@@ -2302,7 +2307,7 @@
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="2">
+      <c r="A157" s="4">
         <v>18319.39027777778</v>
       </c>
       <c r="B157">
@@ -2310,7 +2315,7 @@
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="2">
+      <c r="A158" s="4">
         <v>18319.39305555556</v>
       </c>
       <c r="B158">
@@ -2318,7 +2323,7 @@
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="2">
+      <c r="A159" s="4">
         <v>18319.396643518521</v>
       </c>
       <c r="B159">
@@ -2326,7 +2331,7 @@
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="2">
+      <c r="A160" s="4">
         <v>18319.399421296301</v>
       </c>
       <c r="B160">
@@ -2334,7 +2339,7 @@
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="2">
+      <c r="A161" s="4">
         <v>18319.402777777781</v>
       </c>
       <c r="B161">
@@ -2342,7 +2347,7 @@
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="2">
+      <c r="A162" s="4">
         <v>18319.40532407408</v>
       </c>
       <c r="B162">
@@ -2350,7 +2355,7 @@
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="2">
+      <c r="A163" s="4">
         <v>18319.407407407409</v>
       </c>
       <c r="B163">
@@ -2358,7 +2363,7 @@
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="2">
+      <c r="A164" s="4">
         <v>18319.409490740742</v>
       </c>
       <c r="B164">
@@ -2366,7 +2371,7 @@
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="2">
+      <c r="A165" s="4">
         <v>18319.413541666669</v>
       </c>
       <c r="B165">
@@ -2374,7 +2379,7 @@
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="2">
+      <c r="A166" s="4">
         <v>18319.416666666672</v>
       </c>
       <c r="B166">
@@ -2382,7 +2387,7 @@
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="2">
+      <c r="A167" s="4">
         <v>18319.419328703709</v>
       </c>
       <c r="B167">
@@ -2390,7 +2395,7 @@
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="2">
+      <c r="A168" s="4">
         <v>18319.423611111109</v>
       </c>
       <c r="B168">
@@ -2398,7 +2403,7 @@
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="2">
+      <c r="A169" s="4">
         <v>18319.426388888889</v>
       </c>
       <c r="B169">
@@ -2406,7 +2411,7 @@
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="2">
+      <c r="A170" s="4">
         <v>18319.42905092593</v>
       </c>
       <c r="B170">
@@ -2414,7 +2419,7 @@
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="2">
+      <c r="A171" s="4">
         <v>18319.434375000001</v>
       </c>
       <c r="B171">
@@ -2422,7 +2427,7 @@
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="2">
+      <c r="A172" s="4">
         <v>18319.43715277778</v>
       </c>
       <c r="B172">
@@ -2430,7 +2435,7 @@
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="2">
+      <c r="A173" s="4">
         <v>18319.439467592591</v>
       </c>
       <c r="B173">
@@ -2438,7 +2443,7 @@
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="2">
+      <c r="A174" s="4">
         <v>18319.442361111109</v>
       </c>
       <c r="B174">
@@ -2446,7 +2451,7 @@
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="2">
+      <c r="A175" s="4">
         <v>18319.445370370369</v>
       </c>
       <c r="B175">
@@ -2454,7 +2459,7 @@
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="2">
+      <c r="A176" s="4">
         <v>18319.447800925929</v>
       </c>
       <c r="B176">
@@ -2462,7 +2467,7 @@
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="2">
+      <c r="A177" s="4">
         <v>18319.450462962959</v>
       </c>
       <c r="B177">
@@ -2470,7 +2475,7 @@
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="2">
+      <c r="A178" s="4">
         <v>18319.453356481481</v>
       </c>
       <c r="B178">
@@ -2478,7 +2483,7 @@
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="2">
+      <c r="A179" s="4">
         <v>18319.45648148148</v>
       </c>
       <c r="B179">
@@ -2486,7 +2491,7 @@
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="2">
+      <c r="A180" s="4">
         <v>18319.459027777779</v>
       </c>
       <c r="B180">
@@ -2494,7 +2499,7 @@
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="2">
+      <c r="A181" s="4">
         <v>18319.461342592589</v>
       </c>
       <c r="B181">
@@ -2502,7 +2507,7 @@
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="2">
+      <c r="A182" s="4">
         <v>18319.464120370369</v>
       </c>
       <c r="B182">
@@ -2510,7 +2515,7 @@
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="2">
+      <c r="A183" s="4">
         <v>18319.46643518519</v>
       </c>
       <c r="B183">
@@ -2518,7 +2523,7 @@
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="2">
+      <c r="A184" s="4">
         <v>18319.468865740739</v>
       </c>
       <c r="B184">
@@ -2526,7 +2531,7 @@
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="2">
+      <c r="A185" s="4">
         <v>18319.471874999999</v>
       </c>
       <c r="B185">
@@ -2534,7 +2539,7 @@
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="2">
+      <c r="A186" s="4">
         <v>18319.47789351852</v>
       </c>
       <c r="B186">
@@ -2542,7 +2547,7 @@
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="2">
+      <c r="A187" s="4">
         <v>18319.480787037039</v>
       </c>
       <c r="B187">
@@ -2550,7 +2555,7 @@
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="2">
+      <c r="A188" s="4">
         <v>18319.483912037042</v>
       </c>
       <c r="B188">
@@ -2558,7 +2563,7 @@
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="2">
+      <c r="A189" s="4">
         <v>18319.490740740741</v>
       </c>
       <c r="B189">
@@ -2566,7 +2571,7 @@
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="2">
+      <c r="A190" s="4">
         <v>18319.501273148151</v>
       </c>
       <c r="B190">
@@ -2574,7 +2579,7 @@
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="2">
+      <c r="A191" s="4">
         <v>18319.5037037037</v>
       </c>
       <c r="B191">
@@ -2582,7 +2587,7 @@
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="2">
+      <c r="A192" s="4">
         <v>18319.505671296301</v>
       </c>
       <c r="B192">
@@ -2590,7 +2595,7 @@
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="2">
+      <c r="A193" s="4">
         <v>18319.51423611111</v>
       </c>
       <c r="B193">
@@ -2598,7 +2603,7 @@
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="2">
+      <c r="A194" s="4">
         <v>18319.51805555556</v>
       </c>
       <c r="B194">
@@ -2606,7 +2611,7 @@
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="2">
+      <c r="A195" s="4">
         <v>18319.53055555555</v>
       </c>
       <c r="B195">
@@ -2614,7 +2619,7 @@
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="2">
+      <c r="A196" s="4">
         <v>18319.652777777781</v>
       </c>
       <c r="B196">
@@ -2622,7 +2627,7 @@
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="2">
+      <c r="A197" s="4">
         <v>18319.65694444445</v>
       </c>
       <c r="B197">
@@ -2630,7 +2635,7 @@
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="2">
+      <c r="A198" s="4">
         <v>18319.661226851851</v>
       </c>
       <c r="B198">
@@ -2638,7 +2643,7 @@
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="2">
+      <c r="A199" s="4">
         <v>18319.66435185185</v>
       </c>
       <c r="B199">
@@ -2646,7 +2651,7 @@
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="2">
+      <c r="A200" s="4">
         <v>18319.668287037039</v>
       </c>
       <c r="B200">
@@ -2654,7 +2659,7 @@
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="2">
+      <c r="A201" s="4">
         <v>18319.677083333328</v>
       </c>
       <c r="B201">
@@ -2662,7 +2667,7 @@
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="2">
+      <c r="A202" s="4">
         <v>18319.685879629629</v>
       </c>
       <c r="B202">
@@ -2670,7 +2675,7 @@
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="2">
+      <c r="A203" s="4">
         <v>18319.691666666669</v>
       </c>
       <c r="B203">
@@ -2678,7 +2683,7 @@
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="2">
+      <c r="A204" s="4">
         <v>18319.694444444449</v>
       </c>
       <c r="B204">
@@ -2686,7 +2691,7 @@
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="2">
+      <c r="A205" s="4">
         <v>18319.69768518519</v>
       </c>
       <c r="B205">
@@ -2694,7 +2699,7 @@
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="2">
+      <c r="A206" s="4">
         <v>18319.755555555559</v>
       </c>
       <c r="B206">
@@ -2702,7 +2707,7 @@
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="2">
+      <c r="A207" s="4">
         <v>18319.804861111112</v>
       </c>
       <c r="B207">
@@ -2710,7 +2715,7 @@
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="2">
+      <c r="A208" s="4">
         <v>18319.808217592588</v>
       </c>
       <c r="B208">
@@ -2718,7 +2723,7 @@
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="2">
+      <c r="A209" s="4">
         <v>18319.810532407409</v>
       </c>
       <c r="B209">
@@ -2726,7 +2731,7 @@
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="2">
+      <c r="A210" s="4">
         <v>18319.812731481481</v>
       </c>
       <c r="B210">
@@ -2734,7 +2739,7 @@
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="2">
+      <c r="A211" s="4">
         <v>18319.8162037037</v>
       </c>
       <c r="B211">
@@ -2742,7 +2747,7 @@
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="2">
+      <c r="A212" s="4">
         <v>18319.85185185185</v>
       </c>
       <c r="B212">
@@ -2750,7 +2755,7 @@
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="2">
+      <c r="A213" s="4">
         <v>18319.85706018519</v>
       </c>
       <c r="B213">
@@ -2758,7 +2763,7 @@
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="2">
+      <c r="A214" s="4">
         <v>18319.901620370369</v>
       </c>
       <c r="B214">
@@ -2766,7 +2771,7 @@
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="2">
+      <c r="A215" s="4">
         <v>18319.908101851848</v>
       </c>
       <c r="B215">
@@ -2774,7 +2779,7 @@
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="2">
+      <c r="A216" s="4">
         <v>18319.9181712963</v>
       </c>
       <c r="B216">
@@ -2782,7 +2787,7 @@
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="2">
+      <c r="A217" s="4">
         <v>18319.923379629628</v>
       </c>
       <c r="B217">
@@ -2790,7 +2795,7 @@
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="2">
+      <c r="A218" s="4">
         <v>18319.928703703699</v>
       </c>
       <c r="B218">
@@ -2798,7 +2803,7 @@
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="2">
+      <c r="A219" s="4">
         <v>18319.93240740741</v>
       </c>
       <c r="B219">
@@ -2806,7 +2811,7 @@
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="2">
+      <c r="A220" s="4">
         <v>18319.93657407408</v>
       </c>
       <c r="B220">
@@ -2814,7 +2819,7 @@
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="2">
+      <c r="A221" s="4">
         <v>18319.93981481481</v>
       </c>
       <c r="B221">
@@ -2822,7 +2827,7 @@
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="2">
+      <c r="A222" s="4">
         <v>18319.94456018518</v>
       </c>
       <c r="B222">
@@ -2830,7 +2835,7 @@
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="2">
+      <c r="A223" s="4">
         <v>18319.956597222219</v>
       </c>
       <c r="B223">
@@ -2838,7 +2843,7 @@
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="2">
+      <c r="A224" s="4">
         <v>18319.97106481481</v>
       </c>
       <c r="B224">
@@ -2846,7 +2851,7 @@
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="2">
+      <c r="A225" s="4">
         <v>18319.974074074071</v>
       </c>
       <c r="B225">
@@ -2854,7 +2859,7 @@
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="2">
+      <c r="A226" s="4">
         <v>18319.97592592593</v>
       </c>
       <c r="B226">
@@ -2862,7 +2867,7 @@
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="2">
+      <c r="A227" s="4">
         <v>18319.977777777782</v>
       </c>
       <c r="B227">
@@ -2870,7 +2875,7 @@
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="2">
+      <c r="A228" s="4">
         <v>18320.029629629629</v>
       </c>
       <c r="B228">
@@ -2878,7 +2883,7 @@
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="2">
+      <c r="A229" s="4">
         <v>18320.032523148151</v>
       </c>
       <c r="B229">
@@ -2886,7 +2891,7 @@
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="2">
+      <c r="A230" s="4">
         <v>18320.036226851851</v>
       </c>
       <c r="B230">
@@ -2894,7 +2899,7 @@
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="2">
+      <c r="A231" s="4">
         <v>18320.04212962963</v>
       </c>
       <c r="B231">
@@ -2902,7 +2907,7 @@
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="2">
+      <c r="A232" s="4">
         <v>18321.740393518521</v>
       </c>
       <c r="B232">
@@ -2910,7 +2915,7 @@
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="2">
+      <c r="A233" s="4">
         <v>18321.909722222219</v>
       </c>
       <c r="B233">
@@ -2918,7 +2923,7 @@
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="2">
+      <c r="A234" s="4">
         <v>18322.12638888889</v>
       </c>
       <c r="B234">
@@ -2926,7 +2931,7 @@
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="2">
+      <c r="A235" s="4">
         <v>18322.145486111109</v>
       </c>
       <c r="B235">
@@ -2934,7 +2939,7 @@
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="2">
+      <c r="A236" s="4">
         <v>18322.163888888888</v>
       </c>
       <c r="B236">
@@ -2942,7 +2947,7 @@
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="2">
+      <c r="A237" s="4">
         <v>18322.203356481481</v>
       </c>
       <c r="B237">
@@ -2950,7 +2955,7 @@
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="2">
+      <c r="A238" s="4">
         <v>18322.204861111109</v>
       </c>
       <c r="B238">
@@ -2958,7 +2963,7 @@
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="2">
+      <c r="A239" s="4">
         <v>18322.209837962961</v>
       </c>
       <c r="B239">
@@ -2966,7 +2971,7 @@
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="2">
+      <c r="A240" s="4">
         <v>18322.21168981482</v>
       </c>
       <c r="B240">
@@ -2974,7 +2979,7 @@
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="2">
+      <c r="A241" s="4">
         <v>18322.213888888891</v>
       </c>
       <c r="B241">
@@ -2982,7 +2987,7 @@
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="2">
+      <c r="A242" s="4">
         <v>18322.21597222222</v>
       </c>
       <c r="B242">
@@ -2990,7 +2995,7 @@
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="2">
+      <c r="A243" s="4">
         <v>18322.226388888888</v>
       </c>
       <c r="B243">
@@ -2998,7 +3003,7 @@
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="2">
+      <c r="A244" s="4">
         <v>18322.914004629631</v>
       </c>
       <c r="B244">
@@ -3006,7 +3011,7 @@
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="2">
+      <c r="A245" s="4">
         <v>18322.920601851849</v>
       </c>
       <c r="B245">
@@ -3014,7 +3019,7 @@
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="2">
+      <c r="A246" s="4">
         <v>18322.92627314815</v>
       </c>
       <c r="B246">
@@ -3022,7 +3027,7 @@
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="2">
+      <c r="A247" s="4">
         <v>18322.92997685185</v>
       </c>
       <c r="B247">
@@ -3030,7 +3035,7 @@
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="2">
+      <c r="A248" s="4">
         <v>18322.933217592588</v>
       </c>
       <c r="B248">
@@ -3038,7 +3043,7 @@
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="2">
+      <c r="A249" s="4">
         <v>18322.935995370372</v>
       </c>
       <c r="B249">
@@ -3046,7 +3051,7 @@
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="2">
+      <c r="A250" s="4">
         <v>18322.938657407409</v>
       </c>
       <c r="B250">
@@ -3054,7 +3059,7 @@
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="2">
+      <c r="A251" s="4">
         <v>18322.942013888889</v>
       </c>
       <c r="B251">
@@ -3062,7 +3067,7 @@
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="2">
+      <c r="A252" s="4">
         <v>18322.944328703699</v>
       </c>
       <c r="B252">
@@ -3070,7 +3075,7 @@
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="2">
+      <c r="A253" s="4">
         <v>18322.945833333331</v>
       </c>
       <c r="B253">
@@ -3078,7 +3083,7 @@
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="2">
+      <c r="A254" s="4">
         <v>18322.947569444441</v>
       </c>
       <c r="B254">
@@ -3086,7 +3091,7 @@
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="2">
+      <c r="A255" s="4">
         <v>18322.949189814819</v>
       </c>
       <c r="B255">
@@ -3094,7 +3099,7 @@
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="2">
+      <c r="A256" s="4">
         <v>18322.951273148152</v>
       </c>
       <c r="B256">
@@ -3102,7 +3107,7 @@
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="2">
+      <c r="A257" s="4">
         <v>18322.952893518519</v>
       </c>
       <c r="B257">
@@ -3110,7 +3115,7 @@
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="2">
+      <c r="A258" s="4">
         <v>18322.954398148151</v>
       </c>
       <c r="B258">
@@ -3118,7 +3123,7 @@
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="2">
+      <c r="A259" s="4">
         <v>18322.955671296291</v>
       </c>
       <c r="B259">
@@ -3126,7 +3131,7 @@
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="2">
+      <c r="A260" s="4">
         <v>18322.956944444439</v>
       </c>
       <c r="B260">
@@ -3134,7 +3139,7 @@
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="2">
+      <c r="A261" s="4">
         <v>18322.958101851851</v>
       </c>
       <c r="B261">
@@ -3142,7 +3147,7 @@
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="2">
+      <c r="A262" s="4">
         <v>18322.959722222218</v>
       </c>
       <c r="B262">
@@ -3150,7 +3155,7 @@
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="2">
+      <c r="A263" s="4">
         <v>18322.96122685185</v>
       </c>
       <c r="B263">
@@ -3158,7 +3163,7 @@
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="2">
+      <c r="A264" s="4">
         <v>18322.962847222221</v>
       </c>
       <c r="B264">
@@ -3166,7 +3171,7 @@
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="2">
+      <c r="A265" s="4">
         <v>18322.964583333331</v>
       </c>
       <c r="B265">
@@ -3174,7 +3179,7 @@
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="2">
+      <c r="A266" s="4">
         <v>18322.966550925921</v>
       </c>
       <c r="B266">
@@ -3182,7 +3187,7 @@
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="2">
+      <c r="A267" s="4">
         <v>18322.96909722222</v>
       </c>
       <c r="B267">
@@ -3190,7 +3195,7 @@
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="2">
+      <c r="A268" s="4">
         <v>18322.972800925931</v>
       </c>
       <c r="B268">
@@ -3198,7 +3203,7 @@
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="2">
+      <c r="A269" s="4">
         <v>18323.01284722222</v>
       </c>
       <c r="B269">
@@ -3206,7 +3211,7 @@
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="2">
+      <c r="A270" s="4">
         <v>18323.019097222219</v>
       </c>
       <c r="B270">
@@ -3214,7 +3219,7 @@
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="2">
+      <c r="A271" s="4">
         <v>18323.041550925929</v>
       </c>
       <c r="B271">
@@ -3222,7 +3227,7 @@
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="2">
+      <c r="A272" s="4">
         <v>18323.048611111109</v>
       </c>
       <c r="B272">
@@ -3230,7 +3235,7 @@
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="2">
+      <c r="A273" s="4">
         <v>18323.05</v>
       </c>
       <c r="B273">
@@ -3238,7 +3243,7 @@
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="2">
+      <c r="A274" s="4">
         <v>18323.05127314815</v>
       </c>
       <c r="B274">
@@ -3246,7 +3251,7 @@
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="2">
+      <c r="A275" s="4">
         <v>18323.056828703699</v>
       </c>
       <c r="B275">
@@ -3254,7 +3259,7 @@
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="2">
+      <c r="A276" s="4">
         <v>18323.060879629629</v>
       </c>
       <c r="B276">
@@ -3262,7 +3267,7 @@
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="2">
+      <c r="A277" s="4">
         <v>18323.062962962958</v>
       </c>
       <c r="B277">
@@ -3270,7 +3275,7 @@
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2">
+      <c r="A278" s="4">
         <v>18323.06481481481</v>
       </c>
       <c r="B278">
@@ -3278,7 +3283,7 @@
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="2">
+      <c r="A279" s="4">
         <v>18323.066782407412</v>
       </c>
       <c r="B279">
@@ -3286,7 +3291,7 @@
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="2">
+      <c r="A280" s="4">
         <v>18323.06863425926</v>
       </c>
       <c r="B280">
@@ -3294,7 +3299,7 @@
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="2">
+      <c r="A281" s="4">
         <v>18323.069328703699</v>
       </c>
       <c r="B281">
@@ -3302,7 +3307,7 @@
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="2">
+      <c r="A282" s="4">
         <v>18323.070254629631</v>
       </c>
       <c r="B282">
@@ -3310,7 +3315,7 @@
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="2">
+      <c r="A283" s="4">
         <v>18323.07164351852</v>
       </c>
       <c r="B283">
@@ -3318,7 +3323,7 @@
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="2">
+      <c r="A284" s="4">
         <v>18323.074305555561</v>
       </c>
       <c r="B284">
@@ -3326,7 +3331,7 @@
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="2">
+      <c r="A285" s="4">
         <v>18323.082986111109</v>
       </c>
       <c r="B285">
@@ -3334,7 +3339,7 @@
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="2">
+      <c r="A286" s="4">
         <v>18323.08391203704</v>
       </c>
       <c r="B286">
@@ -3342,7 +3347,7 @@
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="2">
+      <c r="A287" s="4">
         <v>18323.08518518518</v>
       </c>
       <c r="B287">
@@ -3350,7 +3355,7 @@
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="2">
+      <c r="A288" s="4">
         <v>18323.091782407409</v>
       </c>
       <c r="B288">
@@ -3358,7 +3363,7 @@
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="2">
+      <c r="A289" s="4">
         <v>18323.092476851849</v>
       </c>
       <c r="B289">
@@ -3366,7 +3371,7 @@
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="2">
+      <c r="A290" s="4">
         <v>18323.093634259261</v>
       </c>
       <c r="B290">
@@ -3374,7 +3379,7 @@
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="2">
+      <c r="A291" s="4">
         <v>18323.09513888889</v>
       </c>
       <c r="B291">
@@ -3382,7 +3387,7 @@
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="2">
+      <c r="A292" s="4">
         <v>18323.09710648148</v>
       </c>
       <c r="B292">
@@ -3390,7 +3395,7 @@
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="2">
+      <c r="A293" s="4">
         <v>18323.098958333328</v>
       </c>
       <c r="B293">
@@ -3398,7 +3403,7 @@
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="2">
+      <c r="A294" s="4">
         <v>18323.1056712963</v>
       </c>
       <c r="B294">
@@ -3406,7 +3411,7 @@
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="2">
+      <c r="A295" s="4">
         <v>18323.106828703709</v>
       </c>
       <c r="B295">
@@ -3414,7 +3419,7 @@
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="2">
+      <c r="A296" s="4">
         <v>18323.120949074069</v>
       </c>
       <c r="B296">
@@ -3422,7 +3427,7 @@
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="2">
+      <c r="A297" s="4">
         <v>18323.122800925921</v>
       </c>
       <c r="B297">
@@ -3430,7 +3435,7 @@
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="2">
+      <c r="A298" s="4">
         <v>18323.12743055556</v>
       </c>
       <c r="B298">
@@ -3438,7 +3443,7 @@
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="2">
+      <c r="A299" s="4">
         <v>18323.12939814815</v>
       </c>
       <c r="B299">
@@ -3446,7 +3451,7 @@
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="2">
+      <c r="A300" s="4">
         <v>18323.130671296301</v>
       </c>
       <c r="B300">
@@ -3454,7 +3459,7 @@
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="2">
+      <c r="A301" s="4">
         <v>18323.131597222218</v>
       </c>
       <c r="B301">
@@ -3462,7 +3467,7 @@
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="2">
+      <c r="A302" s="4">
         <v>18323.135648148149</v>
       </c>
       <c r="B302">
@@ -3470,7 +3475,7 @@
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="2">
+      <c r="A303" s="4">
         <v>18323.13969907408</v>
       </c>
       <c r="B303">
@@ -3478,7 +3483,7 @@
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="2">
+      <c r="A304" s="4">
         <v>18323.143287037041</v>
       </c>
       <c r="B304">
@@ -3486,7 +3491,7 @@
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="2">
+      <c r="A305" s="4">
         <v>18323.14907407407</v>
       </c>
       <c r="B305">
@@ -3494,7 +3499,7 @@
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="2">
+      <c r="A306" s="4">
         <v>18323.157407407409</v>
       </c>
       <c r="B306">
@@ -3502,7 +3507,7 @@
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="2">
+      <c r="A307" s="4">
         <v>18323.16064814815</v>
       </c>
       <c r="B307">
@@ -3510,7 +3515,7 @@
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="2">
+      <c r="A308" s="4">
         <v>18323.165046296301</v>
       </c>
       <c r="B308">
@@ -3518,7 +3523,7 @@
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="2">
+      <c r="A309" s="4">
         <v>18323.169791666671</v>
       </c>
       <c r="B309">
@@ -3526,7 +3531,7 @@
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="2">
+      <c r="A310" s="4">
         <v>18323.18206018519</v>
       </c>
       <c r="B310">
@@ -3534,7 +3539,7 @@
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="2">
+      <c r="A311" s="4">
         <v>18323.190624999999</v>
       </c>
       <c r="B311">
@@ -3542,7 +3547,7 @@
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" s="2">
+      <c r="A312" s="4">
         <v>18323.193055555559</v>
       </c>
       <c r="B312">
@@ -3550,7 +3555,7 @@
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" s="2">
+      <c r="A313" s="4">
         <v>18323.194791666669</v>
       </c>
       <c r="B313">
@@ -3558,7 +3563,7 @@
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" s="2">
+      <c r="A314" s="4">
         <v>18323.196759259259</v>
       </c>
       <c r="B314">
@@ -3566,7 +3571,7 @@
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="2">
+      <c r="A315" s="4">
         <v>18323.200231481482</v>
       </c>
       <c r="B315">
@@ -3574,7 +3579,7 @@
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" s="2">
+      <c r="A316" s="4">
         <v>18323.203240740739</v>
       </c>
       <c r="B316">
@@ -3582,7 +3587,7 @@
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="2">
+      <c r="A317" s="4">
         <v>18323.207175925931</v>
       </c>
       <c r="B317">
@@ -3590,7 +3595,7 @@
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="2">
+      <c r="A318" s="4">
         <v>18323.210069444449</v>
       </c>
       <c r="B318">
@@ -3598,7 +3603,7 @@
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="2">
+      <c r="A319" s="4">
         <v>18323.21261574074</v>
       </c>
       <c r="B319">
@@ -3606,7 +3611,7 @@
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="2">
+      <c r="A320" s="4">
         <v>18323.214467592588</v>
       </c>
       <c r="B320">
@@ -3614,7 +3619,7 @@
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="2">
+      <c r="A321" s="4">
         <v>18323.21597222222</v>
       </c>
       <c r="B321">
@@ -3622,7 +3627,7 @@
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="2">
+      <c r="A322" s="4">
         <v>18323.21805555555</v>
       </c>
       <c r="B322">
@@ -3630,7 +3635,7 @@
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="2">
+      <c r="A323" s="4">
         <v>18323.219560185189</v>
       </c>
       <c r="B323">
@@ -3638,7 +3643,7 @@
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="2">
+      <c r="A324" s="4">
         <v>18323.221296296291</v>
       </c>
       <c r="B324">
@@ -3646,7 +3651,7 @@
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="2">
+      <c r="A325" s="4">
         <v>18323.22349537037</v>
       </c>
       <c r="B325">
@@ -3654,7 +3659,7 @@
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="2">
+      <c r="A326" s="4">
         <v>18323.225578703699</v>
       </c>
       <c r="B326">
@@ -3662,7 +3667,7 @@
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="2">
+      <c r="A327" s="4">
         <v>18323.228819444441</v>
       </c>
       <c r="B327">
@@ -3670,7 +3675,7 @@
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="2">
+      <c r="A328" s="4">
         <v>18323.231828703709</v>
       </c>
       <c r="B328">
@@ -3678,7 +3683,7 @@
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="2">
+      <c r="A329" s="4">
         <v>18323.237962962961</v>
       </c>
       <c r="B329">
@@ -3686,7 +3691,7 @@
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="2">
+      <c r="A330" s="4">
         <v>18323.41481481482</v>
       </c>
       <c r="B330">
@@ -3694,7 +3699,7 @@
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="2">
+      <c r="A331" s="4">
         <v>18323.492013888888</v>
       </c>
       <c r="B331">
@@ -3702,7 +3707,7 @@
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="2">
+      <c r="A332" s="4">
         <v>18323.49560185185</v>
       </c>
       <c r="B332">
@@ -3710,7 +3715,7 @@
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="2">
+      <c r="A333" s="4">
         <v>18323.49756944444</v>
       </c>
       <c r="B333">
@@ -3718,7 +3723,7 @@
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="2">
+      <c r="A334" s="4">
         <v>18323.498842592591</v>
       </c>
       <c r="B334">
@@ -3726,7 +3731,7 @@
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="2">
+      <c r="A335" s="4">
         <v>18323.50069444445</v>
       </c>
       <c r="B335">
@@ -3734,7 +3739,7 @@
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="2">
+      <c r="A336" s="4">
         <v>18323.501967592591</v>
       </c>
       <c r="B336">
@@ -3742,7 +3747,7 @@
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" s="2">
+      <c r="A337" s="4">
         <v>18323.503819444439</v>
       </c>
       <c r="B337">
@@ -3750,7 +3755,7 @@
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" s="2">
+      <c r="A338" s="4">
         <v>18323.50914351852</v>
       </c>
       <c r="B338">
@@ -3758,7 +3763,7 @@
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" s="2">
+      <c r="A339" s="4">
         <v>18323.510763888891</v>
       </c>
       <c r="B339">
@@ -3766,7 +3771,7 @@
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="2">
+      <c r="A340" s="4">
         <v>18323.51284722222</v>
       </c>
       <c r="B340">
@@ -3774,7 +3779,7 @@
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" s="2">
+      <c r="A341" s="4">
         <v>18323.51423611111</v>
       </c>
       <c r="B341">
@@ -3782,7 +3787,7 @@
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" s="2">
+      <c r="A342" s="4">
         <v>18323.515740740739</v>
       </c>
       <c r="B342">
@@ -3790,7 +3795,7 @@
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" s="2">
+      <c r="A343" s="4">
         <v>18323.517476851848</v>
       </c>
       <c r="B343">
@@ -3798,7 +3803,7 @@
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" s="2">
+      <c r="A344" s="4">
         <v>18323.572569444441</v>
       </c>
       <c r="B344">
@@ -3806,7 +3811,7 @@
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" s="2">
+      <c r="A345" s="4">
         <v>18323.575115740739</v>
       </c>
       <c r="B345">
@@ -3814,7 +3819,7 @@
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" s="2">
+      <c r="A346" s="4">
         <v>18323.57673611111</v>
       </c>
       <c r="B346">

</xml_diff>